<commit_message>
fix problems with the files
</commit_message>
<xml_diff>
--- a/Cojinautos_Clientes.xlsx
+++ b/Cojinautos_Clientes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIVERSIDAD\Bases de datos 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892607C0-CDA3-4737-848F-0F0B3001688C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -216,7 +217,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -277,18 +278,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -307,9 +311,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -347,9 +351,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -384,7 +388,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -419,7 +423,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -592,11 +596,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -609,7 +613,7 @@
     <col min="6" max="6" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -625,307 +629,308 @@
       <c r="E1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="4">
         <v>45301</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="4">
         <v>45337</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="4">
         <v>45371</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="4">
         <v>45407</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="4">
         <v>45442</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="4">
         <v>45453</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="4">
         <v>45488</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="4">
         <v>45505</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="4">
         <v>45509</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="4">
         <v>45514</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="4">
         <v>45342</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="4">
         <v>45376</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="4">
         <v>45412</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="4">
         <v>45422</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="4">
         <v>45458</v>
       </c>
     </row>

</xml_diff>